<commit_message>
Apportate modifiche a SimpleGrid
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/readloocup_output.xlsx
+++ b/src/main/resources/excel/readloocup_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Workspace\ExcelFromXMLObject\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB33A72-BEA9-46E5-BE31-F632F3B080D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153E5EE3-7AE7-455D-9654-28DA0DE0D7B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{D048C21C-6F62-426E-A658-66B2421AE3F1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
   <si>
     <t>Lettura Scheda</t>
   </si>
@@ -42,175 +42,166 @@
     <t>${String}</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>005</t>
   </si>
   <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>-1,12</t>
+  </si>
+  <si>
+    <t>-1,05</t>
+  </si>
+  <si>
+    <t>1,102</t>
+  </si>
+  <si>
+    <t>FIOGIA</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
     <t>2,0</t>
   </si>
   <si>
+    <t>-2,13</t>
+  </si>
+  <si>
+    <t>-2,5</t>
+  </si>
+  <si>
+    <t>2,100</t>
+  </si>
+  <si>
+    <t>SANCOS</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>33,3</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
     <t>-3,14</t>
   </si>
   <si>
-    <t>4-</t>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-3,12541</t>
+  </si>
+  <si>
+    <t>PARFRA</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>-4,15</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>4,40000</t>
+  </si>
+  <si>
+    <t>FORFED</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>-12,16</t>
+  </si>
+  <si>
+    <t>-12</t>
   </si>
   <si>
     <t>12,12000</t>
   </si>
   <si>
+    <t>BELQUI</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>13,4</t>
+  </si>
+  <si>
+    <t>-13,00</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>13.123.213,01200</t>
+  </si>
+  <si>
     <t>ROCMAT</t>
   </si>
   <si>
-    <t>01</t>
+    <t>66</t>
+  </si>
+  <si>
+    <t>14,1</t>
+  </si>
+  <si>
+    <t>-14,01</t>
+  </si>
+  <si>
+    <t>-14</t>
+  </si>
+  <si>
+    <t>1.123.114,49000</t>
+  </si>
+  <si>
+    <t>MAEOLI</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>35,0</t>
+  </si>
+  <si>
+    <t>-35,02</t>
+  </si>
+  <si>
+    <t>-35</t>
+  </si>
+  <si>
+    <t>1.235,35900</t>
+  </si>
+  <si>
+    <t>CARLUC</t>
   </si>
   <si>
     <t>1000</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>-1,12</t>
-  </si>
-  <si>
-    <t>-1,05</t>
-  </si>
-  <si>
-    <t>1,102</t>
-  </si>
-  <si>
-    <t>FIOGIA</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>-2,13</t>
-  </si>
-  <si>
-    <t>-2,5</t>
-  </si>
-  <si>
-    <t>2,100</t>
-  </si>
-  <si>
-    <t>SANCOS</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>33,3</t>
-  </si>
-  <si>
-    <t>3,1</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>-3,12541</t>
-  </si>
-  <si>
-    <t>PARFRA</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>4,2</t>
-  </si>
-  <si>
-    <t>-4,15</t>
-  </si>
-  <si>
-    <t>-4</t>
-  </si>
-  <si>
-    <t>4,40000</t>
-  </si>
-  <si>
-    <t>FORFED</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>-12,16</t>
-  </si>
-  <si>
-    <t>-12</t>
-  </si>
-  <si>
-    <t>BELQUI</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>13,4</t>
-  </si>
-  <si>
-    <t>-13,00</t>
-  </si>
-  <si>
-    <t>-13</t>
-  </si>
-  <si>
-    <t>13.123.213,01200</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>14,1</t>
-  </si>
-  <si>
-    <t>-14,01</t>
-  </si>
-  <si>
-    <t>-14</t>
-  </si>
-  <si>
-    <t>1.123.114,49000</t>
-  </si>
-  <si>
-    <t>MAEOLI</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>35,0</t>
-  </si>
-  <si>
-    <t>-35,02</t>
-  </si>
-  <si>
-    <t>-35</t>
-  </si>
-  <si>
-    <t>1.235,35900</t>
-  </si>
-  <si>
-    <t>CARLUC</t>
   </si>
   <si>
     <t>55</t>
@@ -304,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -312,13 +303,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,17 +341,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{97545357-5703-40BA-8A68-9D9A4D1667C2}" name="Table3" displayName="Table3" ref="A5:B15" totalsRowShown="0">
-  <autoFilter ref="A5:B6" xr:uid="{E84FFCB2-D86E-4E22-9505-1DF7641403AA}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C93CBB3D-9A64-445C-807B-16FF0530B2BE}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{A3840DA8-52D5-4439-9C7E-96D4676E7D78}" name="Column2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,13 +643,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="2" max="2" width="25.0" customWidth="true"/>
     <col min="3" max="3" width="25.0" customWidth="true"/>
     <col min="4" max="4" width="25.0" customWidth="true"/>
     <col min="5" max="5" width="25.0" customWidth="true"/>
@@ -662,313 +658,278 @@
     <col min="8" max="8" width="25.0" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4" customHeight="true">
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4" customHeight="true">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="true"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
-      <c r="A3" s="0" t="s">
+    <row r="3" ht="15.0" customHeight="true"/>
+    <row r="4" ht="15.0" customHeight="true"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="D5" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="E5" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="F5" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="G5" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="H5" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="G3" t="s" s="0">
+    </row>
+    <row r="6" ht="15.0" customHeight="true">
+      <c r="A6" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="B6" t="s" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" ht="15.0" customHeight="true"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
-      <c r="A5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="0">
+      <c r="C6" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="D6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="E6" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="F6" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="G6" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="G6" t="s" s="0">
+      <c r="H6" t="s" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" ht="15.0" customHeight="true">
+      <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H6" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" ht="15.0" customHeight="true">
-      <c r="A7" t="s" s="0">
+      <c r="B7" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="G7" t="s" s="0">
+      <c r="G7" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s" s="2">
         <v>25</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
-      <c r="A8" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s" s="0">
+      <c r="A8" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="B8" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="C8" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="D8" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="G8" t="s" s="0">
+      <c r="E8" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="F8" t="s" s="2">
         <v>31</v>
       </c>
+      <c r="G8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="C9" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="D9" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="E9" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="F9" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="G9" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="G9" t="s" s="0">
+    </row>
+    <row r="10" ht="15.0" customHeight="true">
+      <c r="A10" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" ht="15.0" customHeight="true">
+      <c r="A11" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" ht="15.0" customHeight="true">
+      <c r="A12" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" ht="15.0" customHeight="true">
+      <c r="A13" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H9" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" ht="15.0" customHeight="true">
-      <c r="A10" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="B13" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="F10" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s" s="0">
+      <c r="H13" t="s" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" ht="15.0" customHeight="true">
+      <c r="A14" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H10" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" ht="15.0" customHeight="true">
-      <c r="A11" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" ht="15.0" customHeight="true">
-      <c r="A12" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" ht="15.0" customHeight="true">
-      <c r="A13" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="G13" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" ht="15.0" customHeight="true">
-      <c r="A14" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s" s="0">
+      <c r="B14" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="F14" t="s" s="0">
+      <c r="C14" t="s" s="2">
         <v>63</v>
       </c>
-      <c r="G14" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s" s="0">
+      <c r="D14" t="s" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" ht="15.0" customHeight="true">
-      <c r="A15" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s" s="0">
+      <c r="E14" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="F14" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="G14" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="E15" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="G15" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
+    </row>
+    <row r="15" ht="15.0" customHeight="true"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunte funzionalità a SimpleGrid, creato classe UIToExcelFilter
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/readloocup_output.xlsx
+++ b/src/main/resources/excel/readloocup_output.xlsx
@@ -48,193 +48,193 @@
     <t>005</t>
   </si>
   <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
     <t>1,1</t>
   </si>
   <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13,4</t>
+  </si>
+  <si>
+    <t>14,1</t>
+  </si>
+  <si>
+    <t>35,0</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
     <t>-1,12</t>
   </si>
   <si>
+    <t>-2,13</t>
+  </si>
+  <si>
+    <t>-3,14</t>
+  </si>
+  <si>
+    <t>-4,15</t>
+  </si>
+  <si>
+    <t>-12,16</t>
+  </si>
+  <si>
+    <t>-13,00</t>
+  </si>
+  <si>
+    <t>-14,01</t>
+  </si>
+  <si>
+    <t>-35,02</t>
+  </si>
+  <si>
+    <t>-55,03</t>
+  </si>
+  <si>
+    <t>-121,0</t>
+  </si>
+  <si>
     <t>-1,05</t>
   </si>
   <si>
+    <t>-2,5</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>-12</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>-14</t>
+  </si>
+  <si>
+    <t>-35</t>
+  </si>
+  <si>
+    <t>-55</t>
+  </si>
+  <si>
+    <t>-121</t>
+  </si>
+  <si>
     <t>1,102</t>
   </si>
   <si>
+    <t>2,100</t>
+  </si>
+  <si>
+    <t>-3,12541</t>
+  </si>
+  <si>
+    <t>4,40000</t>
+  </si>
+  <si>
+    <t>12,12000</t>
+  </si>
+  <si>
+    <t>13.123.213,01200</t>
+  </si>
+  <si>
+    <t>1.123.114,49000</t>
+  </si>
+  <si>
+    <t>1.235,35900</t>
+  </si>
+  <si>
+    <t>9.955,00000</t>
+  </si>
+  <si>
+    <t>121,00000</t>
+  </si>
+  <si>
     <t>FIOGIA</t>
   </si>
   <si>
+    <t>SANCOS</t>
+  </si>
+  <si>
+    <t>PARFRA</t>
+  </si>
+  <si>
+    <t>FORFED</t>
+  </si>
+  <si>
+    <t>BELQUI</t>
+  </si>
+  <si>
+    <t>ROCMAT</t>
+  </si>
+  <si>
+    <t>MAEOLI</t>
+  </si>
+  <si>
+    <t>CARLUC</t>
+  </si>
+  <si>
+    <t>CASFRA</t>
+  </si>
+  <si>
+    <t>DELGIO</t>
+  </si>
+  <si>
     <t>01</t>
   </si>
   <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>2,0</t>
-  </si>
-  <si>
-    <t>-2,13</t>
-  </si>
-  <si>
-    <t>-2,5</t>
-  </si>
-  <si>
-    <t>2,100</t>
-  </si>
-  <si>
-    <t>SANCOS</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
     <t>33,3</t>
   </si>
   <si>
-    <t>3,1</t>
-  </si>
-  <si>
-    <t>-3,14</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>-3,12541</t>
-  </si>
-  <si>
-    <t>PARFRA</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>4,2</t>
-  </si>
-  <si>
-    <t>-4,15</t>
-  </si>
-  <si>
-    <t>-4</t>
-  </si>
-  <si>
-    <t>4,40000</t>
-  </si>
-  <si>
-    <t>FORFED</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>-12,16</t>
-  </si>
-  <si>
-    <t>-12</t>
-  </si>
-  <si>
-    <t>12,12000</t>
-  </si>
-  <si>
-    <t>BELQUI</t>
-  </si>
-  <si>
     <t>44</t>
   </si>
   <si>
-    <t>13,4</t>
-  </si>
-  <si>
-    <t>-13,00</t>
-  </si>
-  <si>
-    <t>-13</t>
-  </si>
-  <si>
-    <t>13.123.213,01200</t>
-  </si>
-  <si>
-    <t>ROCMAT</t>
-  </si>
-  <si>
     <t>66</t>
   </si>
   <si>
-    <t>14,1</t>
-  </si>
-  <si>
-    <t>-14,01</t>
-  </si>
-  <si>
-    <t>-14</t>
-  </si>
-  <si>
-    <t>1.123.114,49000</t>
-  </si>
-  <si>
-    <t>MAEOLI</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
-    <t>35,0</t>
-  </si>
-  <si>
-    <t>-35,02</t>
-  </si>
-  <si>
-    <t>-35</t>
-  </si>
-  <si>
-    <t>1.235,35900</t>
-  </si>
-  <si>
-    <t>CARLUC</t>
-  </si>
-  <si>
     <t>1000</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>-55,03</t>
-  </si>
-  <si>
-    <t>-55</t>
-  </si>
-  <si>
-    <t>9.955,00000</t>
-  </si>
-  <si>
-    <t>CASFRA</t>
-  </si>
-  <si>
     <t>55,22</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>-121,0</t>
-  </si>
-  <si>
-    <t>-121</t>
-  </si>
-  <si>
-    <t>121,00000</t>
-  </si>
-  <si>
-    <t>DELGIO</t>
   </si>
   <si>
     <t>20,11</t>
@@ -640,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E2D85D-9821-44E9-A51E-F7E15C655787}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -656,6 +656,8 @@
     <col min="6" max="6" width="25.0" customWidth="true"/>
     <col min="7" max="7" width="25.0" customWidth="true"/>
     <col min="8" max="8" width="25.0" customWidth="true"/>
+    <col min="9" max="9" width="25.0" customWidth="true"/>
+    <col min="10" max="10" width="25.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4" customHeight="true">
@@ -674,73 +676,91 @@
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="D5" t="s" s="2">
-        <v>6</v>
-      </c>
       <c r="E5" t="s" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="G6" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="H6" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="I6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="E6" t="s" s="2">
+      <c r="J6" t="s" s="2">
         <v>15</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>18</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" t="s" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="E7" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="F7" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="E7" t="s" s="2">
+      <c r="G7" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="F7" t="s" s="2">
+      <c r="H7" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="G7" t="s" s="2">
+      <c r="I7" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="H7" t="s" s="2">
+      <c r="J7" t="s" s="2">
         <v>25</v>
       </c>
     </row>
@@ -764,169 +784,147 @@
         <v>31</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" t="s" s="2">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s" s="2">
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" t="s" s="2">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="I10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>55</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" t="s" s="2">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J11" t="s" s="2">
+        <v>56</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" t="s" s="2">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="I12" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>67</v>
       </c>
     </row>
-    <row r="13" ht="15.0" customHeight="true">
-      <c r="A13" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="G13" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" ht="15.0" customHeight="true">
-      <c r="A14" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="E14" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="F14" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" ht="15.0" customHeight="true"/>
+    <row r="13" ht="15.0" customHeight="true"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>